<commit_message>
check1:Patient Needs a Lab Test form
</commit_message>
<xml_diff>
--- a/config/forms/app/check.xlsx
+++ b/config/forms/app/check.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t>type</t>
   </si>
@@ -39,7 +39,7 @@
     <t>inputs</t>
   </si>
   <si>
-    <t>Viral Load test is due</t>
+    <t>Patient Needs a Lab Test</t>
   </si>
   <si>
     <t>./source = 'user'</t>
@@ -117,23 +117,28 @@
     <t>check</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one check </t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
-    <t xml:space="preserve">This patient should have a lab result for the following Lab….
-</t>
-  </si>
-  <si>
-    <t>select_one check or_other</t>
+    <t>Lab test:</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>Lab test:</t>
-  </si>
-  <si>
-    <t>select_one lab</t>
+    <t>Date of Appointment</t>
+  </si>
+  <si>
+    <t>today()</t>
+  </si>
+  <si>
+    <t>select_one result</t>
   </si>
   <si>
     <t>result</t>
@@ -143,48 +148,116 @@
 </t>
   </si>
   <si>
+    <t>select_one count</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viral Load result:
+</t>
+  </si>
+  <si>
+    <t>select_one this</t>
+  </si>
+  <si>
+    <t>should</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This patient should be scheduled for a CD4 Lab count based on their result and date of last lab appointment. 
+</t>
+  </si>
+  <si>
+    <t>select_one lab</t>
+  </si>
+  <si>
+    <t>load2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viral Load:
+</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
+    <t>Viral Load</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unstable - Unsuppressed Viral Load (viral load is above 1,000 copies/ml)
+</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Stable - Suppressed Viral Load (viral load is below 1,000 copies/ml)</t>
+  </si>
+  <si>
+    <t>result1</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>result2</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>result3</t>
+  </si>
+  <si>
+    <t>Unknown  (Lab test did not give a result after 14 days. Close this Task and set up new lab test appointment for patient to get a new lab draw)</t>
+  </si>
+  <si>
     <t>count</t>
   </si>
   <si>
-    <t>CD4 count</t>
-  </si>
-  <si>
-    <t>load</t>
-  </si>
-  <si>
-    <t>Viral Load</t>
-  </si>
-  <si>
-    <t>lab</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No, snooze this task for 2 days
+    <t>count1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable or Suppressed (viral load is below 1,000 copies/ml)
 </t>
   </si>
   <si>
-    <t>draw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown if patient got this blood draw, snooze this task for 2 days
+    <t>count2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unstable or Unsuppressed 
+(viral load is above 1,000 copies/ml)
 </t>
   </si>
   <si>
-    <t>ignore</t>
-  </si>
-  <si>
-    <t>Ignore this task</t>
+    <t>count3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inconclusive (Viral Load Lab test did not work or had an error, so patient will need to repeat this lab test)
+</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>this1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okay, I will schedule an appointment for a lab visit
+</t>
+  </si>
+  <si>
+    <t>this2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep this reminder in my Task List Remind me to schedule an appointment in 2 days 
+</t>
   </si>
   <si>
     <t>form_title</t>
@@ -206,9 +279,6 @@
   </si>
   <si>
     <t>default_language</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Check for Lab Result </t>
   </si>
   <si>
     <t>pages</t>
@@ -307,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -316,6 +386,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -584,7 +657,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="23.13"/>
-    <col customWidth="1" min="3" max="3" width="48.38"/>
+    <col customWidth="1" min="3" max="3" width="80.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -614,7 +687,7 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -626,13 +699,13 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="2"/>
@@ -642,13 +715,13 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2"/>
@@ -658,13 +731,13 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2"/>
@@ -672,13 +745,13 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2"/>
@@ -688,13 +761,13 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2"/>
@@ -704,13 +777,13 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2"/>
@@ -720,13 +793,13 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
@@ -736,13 +809,13 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2"/>
@@ -752,13 +825,13 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
@@ -766,13 +839,13 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2"/>
@@ -780,13 +853,13 @@
       <c r="F12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2"/>
@@ -796,13 +869,13 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2"/>
@@ -812,82 +885,82 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="6"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7" t="s">
+      <c r="E19" s="7"/>
+      <c r="F19" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -897,7 +970,7 @@
       <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -920,40 +993,76 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>35</v>
       </c>
+      <c r="C22" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="C23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="A24" s="12" t="s">
         <v>41</v>
       </c>
+      <c r="B24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -972,12 +1081,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="26.0"/>
+    <col customWidth="1" min="3" max="3" width="107.13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -987,69 +1096,124 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>44</v>
+      <c r="B2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>46</v>
+      <c r="A3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>49</v>
+      <c r="A4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>51</v>
+      <c r="A5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>53</v>
+      <c r="A6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>55</v>
+      <c r="A7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1067,52 +1231,52 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="1" max="1" width="22.25"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>62</v>
+      <c r="A1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="15" t="str">
+      <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-06-30_11-38</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
-        <v>66</v>
+        <v>2022-07-13_17-36</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>